<commit_message>
Haziran Ve Temmuz Aylarından Kalanlar Eklendi.
</commit_message>
<xml_diff>
--- a/Ofis Dosyalari/HAKEDISLER/2025/AĞUSTOS 2025/2025 AĞUSTOS AYI - AVTADOR.xlsx
+++ b/Ofis Dosyalari/HAKEDISLER/2025/AĞUSTOS 2025/2025 AĞUSTOS AYI - AVTADOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samil\OneDrive\Desktop\OfisDosyalariYedegi\Ofis Dosyalari\HAKEDISLER\2025\AĞUSTOS 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178A2079-968D-447F-873F-F0C4F7417646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED8FBAA-0C71-44AB-A35D-1F6E10E3DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>№</t>
   </si>
@@ -107,9 +107,6 @@
     <t>TURSUNALIYEV ALISER</t>
   </si>
   <si>
-    <t>MAMASIDIKOV MAHMUDJON</t>
-  </si>
-  <si>
     <t>ISMATILLO ERGASOV</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>SOLIEV ABDUVALI</t>
   </si>
   <si>
-    <t>TURSUNALIEV BUNYODJON</t>
-  </si>
-  <si>
     <t>TURSUNOV KOMILJON</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
   </si>
   <si>
     <t>YYP AĞUSTOS</t>
-  </si>
-  <si>
-    <t>AGREGADAN PARA VERILDI MI BAK</t>
   </si>
 </sst>
 </file>
@@ -229,7 +220,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,17 +544,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -700,9 +682,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1013,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1025,665 +1013,605 @@
     <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="52"/>
+    </row>
+    <row r="2" spans="1:11" ht="29.4" thickBot="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="29.4" thickBot="1">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10">
         <v>200000</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12">
         <f>F3-G3-H3-I3</f>
         <v>200000</v>
       </c>
-      <c r="K3" s="16"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1">
-      <c r="A4" s="17">
+      <c r="A4" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22">
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19">
         <v>200000</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23">
+      <c r="G4" s="18"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20">
         <v>24900</v>
       </c>
-      <c r="J4" s="24">
-        <f t="shared" ref="J4:J22" si="0">F4-G4-H4-I4</f>
+      <c r="J4" s="21">
+        <f t="shared" ref="J4:J20" si="0">F4-G4-H4-I4</f>
         <v>175100</v>
       </c>
-      <c r="K4" s="25"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1">
-      <c r="A5" s="17">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22">
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19">
         <v>100000</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="23">
+      <c r="G5" s="18"/>
+      <c r="H5" s="20">
         <v>15000</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="20">
         <v>15000</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="21">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="K5" s="25"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1">
-      <c r="A6" s="28">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="26">
         <v>188</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="20">
         <v>450</v>
       </c>
-      <c r="F6" s="30">
-        <f t="shared" ref="F6:F22" si="1">D6*E6</f>
+      <c r="F6" s="27">
+        <f t="shared" ref="F6:F20" si="1">D6*E6</f>
         <v>84600</v>
       </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="24">
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="21">
         <f t="shared" si="0"/>
         <v>84600</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1">
-      <c r="A7" s="17">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="30">
         <v>124</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="26">
         <v>348</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>330</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="27">
         <f t="shared" si="1"/>
         <v>114840</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="28">
         <v>25000</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="24">
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="21">
         <f t="shared" si="0"/>
         <v>89840</v>
       </c>
-      <c r="K7" s="32"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="17">
+      <c r="A8" s="14">
         <v>6</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="32">
         <v>144</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="26">
         <v>345</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="20">
         <v>380</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="27">
         <f t="shared" si="1"/>
         <v>131100</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="28">
         <v>25000</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="24">
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="21">
         <f t="shared" si="0"/>
         <v>106100</v>
       </c>
-      <c r="K8" s="32"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="28">
+      <c r="A9" s="25">
         <v>7</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="15">
         <v>159</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="26">
         <v>357</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="20">
         <v>410</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="27">
         <f t="shared" si="1"/>
         <v>146370</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="28">
         <v>25000</v>
       </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="24">
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="21">
         <f t="shared" si="0"/>
         <v>121370</v>
       </c>
-      <c r="K9" s="32"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1">
-      <c r="A10" s="17">
+      <c r="A10" s="14">
         <v>8</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="15">
         <v>174</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="26">
         <v>333</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="20">
         <v>410</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="27">
         <f t="shared" si="1"/>
         <v>136530</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="28">
         <v>25000</v>
       </c>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="24">
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="21">
         <f t="shared" si="0"/>
         <v>111530</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1">
-      <c r="A11" s="17">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="35">
         <v>198</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="26">
         <v>341</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="20">
         <v>400</v>
       </c>
-      <c r="F11" s="30">
+      <c r="F11" s="27">
         <f t="shared" si="1"/>
         <v>136400</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="28">
         <v>25000</v>
       </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="24">
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="21">
         <f t="shared" si="0"/>
         <v>111400</v>
       </c>
-      <c r="K11" s="32"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1">
-      <c r="A12" s="28">
+      <c r="A12" s="25">
         <v>10</v>
       </c>
-      <c r="B12" s="39">
+      <c r="B12" s="36">
         <v>210</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="26">
         <v>279</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="20">
         <v>380</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="27">
         <f t="shared" si="1"/>
         <v>106020</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="28">
         <v>25000</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="24">
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="21">
         <f t="shared" si="0"/>
         <v>81020</v>
       </c>
-      <c r="K12" s="32"/>
+      <c r="K12" s="29"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1">
-      <c r="A13" s="17">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
-      <c r="B13" s="40">
-        <v>219</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="B13" s="38">
+        <v>285</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="29">
-        <v>345</v>
-      </c>
-      <c r="E13" s="23">
-        <v>380</v>
-      </c>
-      <c r="F13" s="30">
-        <f t="shared" si="1"/>
-        <v>131100</v>
-      </c>
-      <c r="G13" s="31">
-        <v>25000</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="24">
-        <f t="shared" si="0"/>
-        <v>106100</v>
-      </c>
-      <c r="K13" s="32"/>
-    </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1">
-      <c r="A14" s="17">
-        <v>12</v>
-      </c>
-      <c r="B14" s="41">
-        <v>285</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="29">
+      <c r="D13" s="26">
         <v>321</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E13" s="20">
         <v>350</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F13" s="27">
         <f t="shared" si="1"/>
         <v>112350</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G13" s="28">
         <v>25000</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="24">
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="21">
         <f t="shared" si="0"/>
         <v>87350</v>
       </c>
-      <c r="K14" s="32"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1">
-      <c r="A15" s="28">
-        <v>13</v>
-      </c>
-      <c r="B15" s="41">
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1">
+      <c r="A14" s="14">
+        <v>12</v>
+      </c>
+      <c r="B14" s="38">
         <v>305</v>
       </c>
-      <c r="C15" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="29">
+      <c r="C14" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="26">
         <v>299</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E14" s="20">
         <v>380</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F14" s="27">
         <f t="shared" si="1"/>
         <v>113620</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G14" s="28">
         <v>25000</v>
       </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="24">
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="21">
         <f t="shared" si="0"/>
         <v>88620</v>
       </c>
-      <c r="K15" s="32"/>
-    </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="17">
-        <v>14</v>
-      </c>
-      <c r="B16" s="40">
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1">
+      <c r="A15" s="25">
+        <v>13</v>
+      </c>
+      <c r="B15" s="37">
         <v>310</v>
       </c>
-      <c r="C16" s="37" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="29">
+      <c r="C15" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="26">
         <v>321</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E15" s="20">
         <v>400</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F15" s="27">
         <f t="shared" si="1"/>
         <v>128400</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G15" s="28">
         <v>25000</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="24">
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="21">
         <f t="shared" si="0"/>
         <v>103400</v>
       </c>
-      <c r="K16" s="32"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1">
-      <c r="A17" s="17">
-        <v>15</v>
-      </c>
-      <c r="B17" s="40">
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1">
+      <c r="A16" s="14">
+        <v>14</v>
+      </c>
+      <c r="B16" s="37">
         <v>315</v>
       </c>
-      <c r="C17" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="29">
+      <c r="C16" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="26">
         <v>345</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E16" s="20">
         <v>400</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F16" s="27">
         <f t="shared" si="1"/>
         <v>138000</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G16" s="28">
         <v>25000</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="24">
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="21">
         <f t="shared" si="0"/>
         <v>113000</v>
       </c>
-      <c r="K17" s="32"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1">
-      <c r="A18" s="53">
-        <v>16</v>
-      </c>
-      <c r="B18" s="54">
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1">
+      <c r="A17" s="14">
+        <v>15</v>
+      </c>
+      <c r="B17" s="53">
         <v>337</v>
       </c>
-      <c r="C18" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="56">
+      <c r="C17" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="55">
         <v>310</v>
       </c>
-      <c r="E18" s="57">
+      <c r="E17" s="56">
         <v>380</v>
       </c>
-      <c r="F18" s="58">
+      <c r="F17" s="57">
         <f t="shared" si="1"/>
         <v>117800</v>
       </c>
-      <c r="G18" s="59">
+      <c r="G17" s="58">
         <v>25000</v>
       </c>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="60">
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="59">
         <f t="shared" si="0"/>
         <v>92800</v>
       </c>
-      <c r="K18" s="61"/>
-      <c r="L18" s="52" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1">
-      <c r="A19" s="17">
-        <v>17</v>
-      </c>
-      <c r="B19" s="40">
+      <c r="K17" s="60"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1">
+      <c r="A18" s="25">
+        <v>16</v>
+      </c>
+      <c r="B18" s="37">
         <v>371</v>
       </c>
-      <c r="C19" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="29">
+      <c r="C18" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="26">
         <v>357</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E18" s="20">
         <v>410</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F18" s="27">
         <f t="shared" si="1"/>
         <v>146370</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G18" s="28">
         <v>25000</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="24">
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="21">
         <f t="shared" si="0"/>
         <v>121370</v>
       </c>
-      <c r="K19" s="32"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1">
-      <c r="A20" s="17">
-        <v>18</v>
-      </c>
-      <c r="B20" s="40">
+      <c r="K18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1">
+      <c r="A19" s="14">
+        <v>17</v>
+      </c>
+      <c r="B19" s="37">
         <v>425</v>
       </c>
-      <c r="C20" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="29">
+      <c r="C19" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="26">
         <v>333</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E19" s="20">
         <v>400</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F19" s="27">
         <f t="shared" si="1"/>
         <v>133200</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G19" s="28">
         <v>25000</v>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="24">
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="21">
         <f t="shared" si="0"/>
         <v>108200</v>
       </c>
-      <c r="K20" s="32"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" customHeight="1">
-      <c r="A21" s="28">
-        <v>19</v>
-      </c>
-      <c r="B21" s="40">
-        <v>427</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="29">
-        <v>372</v>
-      </c>
-      <c r="E21" s="23">
-        <v>350</v>
-      </c>
-      <c r="F21" s="30">
-        <f t="shared" si="1"/>
-        <v>130200</v>
-      </c>
-      <c r="G21" s="31">
-        <v>25000</v>
-      </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="24">
-        <f t="shared" si="0"/>
-        <v>105200</v>
-      </c>
-      <c r="K21" s="32"/>
-    </row>
-    <row r="22" spans="1:12" ht="15" customHeight="1" thickBot="1">
-      <c r="A22" s="43">
-        <v>20</v>
-      </c>
-      <c r="B22" s="44">
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" thickBot="1">
+      <c r="A20" s="40">
+        <v>18</v>
+      </c>
+      <c r="B20" s="41">
         <v>429</v>
       </c>
-      <c r="C22" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="46">
+      <c r="C20" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="43">
         <v>357</v>
       </c>
-      <c r="E22" s="47">
+      <c r="E20" s="44">
         <v>400</v>
       </c>
-      <c r="F22" s="48">
+      <c r="F20" s="45">
         <f t="shared" si="1"/>
         <v>142800</v>
       </c>
-      <c r="G22" s="49">
+      <c r="G20" s="46">
         <v>25000</v>
       </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="50">
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="47">
         <f t="shared" si="0"/>
         <v>117800</v>
       </c>
-      <c r="K22" s="51"/>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="J22" s="49">
+        <f>SUM(J3:J21)</f>
+        <v>1983500</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>